<commit_message>
Needs to be modified
</commit_message>
<xml_diff>
--- a/near_at.xlsx
+++ b/near_at.xlsx
@@ -454,7 +454,7 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5">
@@ -776,7 +776,7 @@
         </is>
       </c>
       <c r="E18" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19">
@@ -1006,7 +1006,7 @@
         </is>
       </c>
       <c r="E28" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="29">
@@ -1029,7 +1029,7 @@
         </is>
       </c>
       <c r="E29" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30">
@@ -1098,7 +1098,7 @@
         </is>
       </c>
       <c r="E32" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="33">
@@ -1236,7 +1236,7 @@
         </is>
       </c>
       <c r="E38" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39">
@@ -1259,7 +1259,7 @@
         </is>
       </c>
       <c r="E39" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="40">
@@ -1420,7 +1420,7 @@
         </is>
       </c>
       <c r="E46" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="47">
@@ -1742,7 +1742,7 @@
         </is>
       </c>
       <c r="E60" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="61">
@@ -1857,7 +1857,7 @@
         </is>
       </c>
       <c r="E65" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="66">
@@ -1926,7 +1926,7 @@
         </is>
       </c>
       <c r="E68" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="69">
@@ -2271,7 +2271,7 @@
         </is>
       </c>
       <c r="E83" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="84">
@@ -2961,7 +2961,7 @@
         </is>
       </c>
       <c r="E113" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="114">
@@ -3743,7 +3743,7 @@
         </is>
       </c>
       <c r="E147" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="148">
@@ -4134,7 +4134,7 @@
         </is>
       </c>
       <c r="E164" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="165">
@@ -4410,7 +4410,7 @@
         </is>
       </c>
       <c r="E176" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="177">
@@ -4433,7 +4433,7 @@
         </is>
       </c>
       <c r="E177" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="178">
@@ -4502,7 +4502,7 @@
         </is>
       </c>
       <c r="E180" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="181">
@@ -4732,7 +4732,7 @@
         </is>
       </c>
       <c r="E190" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="191">
@@ -4893,7 +4893,7 @@
         </is>
       </c>
       <c r="E197" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="198">
@@ -5675,7 +5675,7 @@
         </is>
       </c>
       <c r="E231" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="232">
@@ -7193,7 +7193,7 @@
         </is>
       </c>
       <c r="E297" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="298">
@@ -7377,7 +7377,7 @@
         </is>
       </c>
       <c r="E305" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="306">
@@ -7515,7 +7515,7 @@
         </is>
       </c>
       <c r="E311" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="312">
@@ -7584,7 +7584,7 @@
         </is>
       </c>
       <c r="E314" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="315">
@@ -7906,7 +7906,7 @@
         </is>
       </c>
       <c r="E328" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="329">
@@ -7929,7 +7929,7 @@
         </is>
       </c>
       <c r="E329" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="330">
@@ -8251,7 +8251,7 @@
         </is>
       </c>
       <c r="E343" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="344">
@@ -8757,7 +8757,7 @@
         </is>
       </c>
       <c r="E365" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="366">
@@ -9516,7 +9516,7 @@
         </is>
       </c>
       <c r="E398" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="399">
@@ -9746,7 +9746,7 @@
         </is>
       </c>
       <c r="E408" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="409">
@@ -10482,7 +10482,7 @@
         </is>
       </c>
       <c r="E440" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="441">
@@ -10528,7 +10528,7 @@
         </is>
       </c>
       <c r="E442" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="443">
@@ -10551,7 +10551,7 @@
         </is>
       </c>
       <c r="E443" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="444">
@@ -10712,7 +10712,7 @@
         </is>
       </c>
       <c r="E450" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="451">
@@ -11103,7 +11103,7 @@
         </is>
       </c>
       <c r="E467" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="468">
@@ -11333,7 +11333,7 @@
         </is>
       </c>
       <c r="E477" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="478">
@@ -11471,7 +11471,7 @@
         </is>
       </c>
       <c r="E483" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="484">
@@ -12552,7 +12552,7 @@
         </is>
       </c>
       <c r="E530" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="531">
@@ -12828,7 +12828,7 @@
         </is>
       </c>
       <c r="E542" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="543">
@@ -13242,7 +13242,7 @@
         </is>
       </c>
       <c r="E560" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="561">
@@ -13288,7 +13288,7 @@
         </is>
       </c>
       <c r="E562" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="563">
@@ -13334,7 +13334,7 @@
         </is>
       </c>
       <c r="E564" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="565">
@@ -13495,7 +13495,7 @@
         </is>
       </c>
       <c r="E571" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="572">
@@ -13633,7 +13633,7 @@
         </is>
       </c>
       <c r="E577" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="578">
@@ -13817,7 +13817,7 @@
         </is>
       </c>
       <c r="E585" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="586">
@@ -14461,7 +14461,7 @@
         </is>
       </c>
       <c r="E613" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="614">
@@ -14553,7 +14553,7 @@
         </is>
       </c>
       <c r="E617" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="618">
@@ -15059,7 +15059,7 @@
         </is>
       </c>
       <c r="E639" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="640">
@@ -15197,7 +15197,7 @@
         </is>
       </c>
       <c r="E645" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="646">
@@ -15289,7 +15289,7 @@
         </is>
       </c>
       <c r="E649" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="650">
@@ -15519,7 +15519,7 @@
         </is>
       </c>
       <c r="E659" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="660">
@@ -15841,7 +15841,7 @@
         </is>
       </c>
       <c r="E673" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="674">
@@ -15933,7 +15933,7 @@
         </is>
       </c>
       <c r="E677" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="678">
@@ -15956,7 +15956,7 @@
         </is>
       </c>
       <c r="E678" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="679">
@@ -16232,7 +16232,7 @@
         </is>
       </c>
       <c r="E690" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="691">
@@ -16853,7 +16853,7 @@
         </is>
       </c>
       <c r="E717" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="718">
@@ -17129,7 +17129,7 @@
         </is>
       </c>
       <c r="E729" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="730">
@@ -17198,7 +17198,7 @@
         </is>
       </c>
       <c r="E732" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="733">
@@ -17750,7 +17750,7 @@
         </is>
       </c>
       <c r="E756" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="757">
@@ -18118,7 +18118,7 @@
         </is>
       </c>
       <c r="E772" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="773">
@@ -18187,7 +18187,7 @@
         </is>
       </c>
       <c r="E775" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="776">
@@ -18532,7 +18532,7 @@
         </is>
       </c>
       <c r="E790" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="791">
@@ -18647,7 +18647,7 @@
         </is>
       </c>
       <c r="E795" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="796">
@@ -19038,7 +19038,7 @@
         </is>
       </c>
       <c r="E812" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="813">
@@ -19429,7 +19429,7 @@
         </is>
       </c>
       <c r="E829" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="830">
@@ -19636,7 +19636,7 @@
         </is>
       </c>
       <c r="E838" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="839">
@@ -19682,7 +19682,7 @@
         </is>
       </c>
       <c r="E840" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="841">
@@ -19705,7 +19705,7 @@
         </is>
       </c>
       <c r="E841" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="842">
@@ -19866,7 +19866,7 @@
         </is>
       </c>
       <c r="E848" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="849">
@@ -20395,7 +20395,7 @@
         </is>
       </c>
       <c r="E871" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="872">
@@ -20533,7 +20533,7 @@
         </is>
       </c>
       <c r="E877" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="878">
@@ -20717,7 +20717,7 @@
         </is>
       </c>
       <c r="E885" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="886">
@@ -21085,7 +21085,7 @@
         </is>
       </c>
       <c r="E901" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="902">
@@ -21108,7 +21108,7 @@
         </is>
       </c>
       <c r="E902" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="903">
@@ -21223,7 +21223,7 @@
         </is>
       </c>
       <c r="E907" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="908">
@@ -21246,7 +21246,7 @@
         </is>
       </c>
       <c r="E908" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="909">
@@ -21338,7 +21338,7 @@
         </is>
       </c>
       <c r="E912" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="913">
@@ -21476,7 +21476,7 @@
         </is>
       </c>
       <c r="E918" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="919">
@@ -21867,7 +21867,7 @@
         </is>
       </c>
       <c r="E935" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="936">
@@ -22143,7 +22143,7 @@
         </is>
       </c>
       <c r="E947" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="948">
@@ -22281,7 +22281,7 @@
         </is>
       </c>
       <c r="E953" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="954">
@@ -22787,7 +22787,7 @@
         </is>
       </c>
       <c r="E975" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="976">
@@ -23040,7 +23040,7 @@
         </is>
       </c>
       <c r="E986" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="987">
@@ -23684,7 +23684,7 @@
         </is>
       </c>
       <c r="E1014" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="1015">
@@ -24972,7 +24972,7 @@
         </is>
       </c>
       <c r="E1070" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1071">
@@ -25271,7 +25271,7 @@
         </is>
       </c>
       <c r="E1083" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="1084">
@@ -25294,7 +25294,7 @@
         </is>
       </c>
       <c r="E1084" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="1085">
@@ -25501,7 +25501,7 @@
         </is>
       </c>
       <c r="E1093" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="1094">
@@ -25547,7 +25547,7 @@
         </is>
       </c>
       <c r="E1095" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="1096">
@@ -25662,7 +25662,7 @@
         </is>
       </c>
       <c r="E1100" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1101">
@@ -26076,7 +26076,7 @@
         </is>
       </c>
       <c r="E1118" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1119">
@@ -26099,7 +26099,7 @@
         </is>
       </c>
       <c r="E1119" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1120">
@@ -26191,7 +26191,7 @@
         </is>
       </c>
       <c r="E1123" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="1124">
@@ -26674,7 +26674,7 @@
         </is>
       </c>
       <c r="E1144" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="1145">
@@ -27019,7 +27019,7 @@
         </is>
       </c>
       <c r="E1159" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="1160">
@@ -27663,7 +27663,7 @@
         </is>
       </c>
       <c r="E1187" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="1188">
@@ -27686,7 +27686,7 @@
         </is>
       </c>
       <c r="E1188" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1189">
@@ -27824,7 +27824,7 @@
         </is>
       </c>
       <c r="E1194" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="1195">
@@ -28031,7 +28031,7 @@
         </is>
       </c>
       <c r="E1203" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="1204">
@@ -28491,7 +28491,7 @@
         </is>
       </c>
       <c r="E1223" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="1224">
@@ -28514,7 +28514,7 @@
         </is>
       </c>
       <c r="E1224" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1225">
@@ -29020,7 +29020,7 @@
         </is>
       </c>
       <c r="E1246" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1247">
@@ -29411,7 +29411,7 @@
         </is>
       </c>
       <c r="E1263" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1264">
@@ -29434,7 +29434,7 @@
         </is>
       </c>
       <c r="E1264" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="1265">
@@ -29687,7 +29687,7 @@
         </is>
       </c>
       <c r="E1275" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1276">
@@ -29779,7 +29779,7 @@
         </is>
       </c>
       <c r="E1279" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="1280">
@@ -29871,7 +29871,7 @@
         </is>
       </c>
       <c r="E1283" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="1284">
@@ -30032,7 +30032,7 @@
         </is>
       </c>
       <c r="E1290" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1291">
@@ -30239,7 +30239,7 @@
         </is>
       </c>
       <c r="E1299" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="1300">
@@ -30285,7 +30285,7 @@
         </is>
       </c>
       <c r="E1301" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1302">
@@ -30400,7 +30400,7 @@
         </is>
       </c>
       <c r="E1306" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="1307">

</xml_diff>